<commit_message>
Add comprehensive documentation for formula-based Excel version
Co-authored-by: peetee09 <93839860+peetee09@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Ecom_Operations_Tracking_System_Formula_Based.xlsx
+++ b/Ecom_Operations_Tracking_System_Formula_Based.xlsx
@@ -928,7 +928,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>45937.23209005229</v>
+        <v>45937.23515745207</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -982,7 +982,7 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>45937.23209005229</v>
+        <v>45937.23515745207</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -1036,7 +1036,7 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>45937.23209005229</v>
+        <v>45937.23515745207</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -1090,7 +1090,7 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>45937.23209005229</v>
+        <v>45937.23515745207</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -1237,7 +1237,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>45937.2320900644</v>
+        <v>45937.23515746477</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -1287,7 +1287,7 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>45937.2320900644</v>
+        <v>45937.23515746477</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -1337,7 +1337,7 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>45937.2320900644</v>
+        <v>45937.23515746477</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -1387,7 +1387,7 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>45937.2320900644</v>
+        <v>45937.23515746477</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -1842,7 +1842,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>45937.23208994648</v>
+        <v>45937.23515733849</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -1870,7 +1870,7 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>45937.23208994648</v>
+        <v>45937.23515733849</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -1898,7 +1898,7 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>45937.23208994648</v>
+        <v>45937.23515733849</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -1926,7 +1926,7 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>45937.23208994648</v>
+        <v>45937.23515733849</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -1954,7 +1954,7 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>45937.23208994648</v>
+        <v>45937.23515733849</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -1982,7 +1982,7 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>45937.23208994648</v>
+        <v>45937.23515733849</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -2010,7 +2010,7 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>45937.23208994648</v>
+        <v>45937.23515733849</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -2125,13 +2125,13 @@
         </is>
       </c>
       <c r="B3" s="9" t="n">
-        <v>45937.19042329207</v>
+        <v>45937.193490685</v>
       </c>
       <c r="C3" s="9" t="n">
-        <v>45937.23208995874</v>
+        <v>45937.23515735166</v>
       </c>
       <c r="D3" s="9" t="n">
-        <v>45937.22861773652</v>
+        <v>45937.23168512945</v>
       </c>
       <c r="E3" s="10">
         <f>(D3-B3)*24*60</f>
@@ -2161,13 +2161,13 @@
         </is>
       </c>
       <c r="B4" s="9" t="n">
-        <v>45937.14875662541</v>
+        <v>45937.15182401834</v>
       </c>
       <c r="C4" s="9" t="n">
-        <v>45937.19042329207</v>
+        <v>45937.193490685</v>
       </c>
       <c r="D4" s="9" t="n">
-        <v>45937.18695106985</v>
+        <v>45937.19001846278</v>
       </c>
       <c r="E4" s="10">
         <f>(D4-B4)*24*60</f>
@@ -2197,10 +2197,10 @@
         </is>
       </c>
       <c r="B5" s="9" t="n">
-        <v>45937.21125662541</v>
+        <v>45937.21432401834</v>
       </c>
       <c r="C5" s="9" t="n">
-        <v>45937.25292329207</v>
+        <v>45937.255990685</v>
       </c>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
@@ -2228,10 +2228,10 @@
         </is>
       </c>
       <c r="B6" s="9" t="n">
-        <v>45937.22167329207</v>
+        <v>45937.224740685</v>
       </c>
       <c r="C6" s="9" t="n">
-        <v>45937.26333995874</v>
+        <v>45937.26640735166</v>
       </c>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
@@ -2752,7 +2752,7 @@
         <v>500</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>45937.12792332399</v>
+        <v>45937.13099071968</v>
       </c>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="n">
@@ -2795,10 +2795,10 @@
         <v>750</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>45937.15708999066</v>
+        <v>45937.16015738634</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>45937.23208999066</v>
+        <v>45937.23515738634</v>
       </c>
       <c r="I4" s="7">
         <f>(H4-G4)*24</f>
@@ -2841,7 +2841,7 @@
         <v>1000</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>45937.09875665732</v>
+        <v>45937.10182405301</v>
       </c>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="n">
@@ -2884,10 +2884,10 @@
         <v>600</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>45937.14458999066</v>
+        <v>45937.14765738634</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>45937.23208999066</v>
+        <v>45937.23515738634</v>
       </c>
       <c r="I6" s="7">
         <f>(H6-G6)*24</f>
@@ -3010,7 +3010,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>45937.23209000367</v>
+        <v>45937.23515740021</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -3055,7 +3055,7 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>45937.23209000367</v>
+        <v>45937.23515740021</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -3100,7 +3100,7 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>45937.23209000367</v>
+        <v>45937.23515740021</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -3145,7 +3145,7 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>45937.23209000367</v>
+        <v>45937.23515740021</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -3299,10 +3299,10 @@
         </is>
       </c>
       <c r="D3" s="2" t="n">
-        <v>45937.21264557135</v>
+        <v>45937.21571296886</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>45937.2320900158</v>
+        <v>45937.2351574133</v>
       </c>
       <c r="F3" t="n">
         <v>45</v>
@@ -3344,10 +3344,10 @@
         </is>
       </c>
       <c r="D4" s="2" t="n">
-        <v>45937.20570112691</v>
+        <v>45937.20876852441</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>45937.2320900158</v>
+        <v>45937.2351574133</v>
       </c>
       <c r="F4" t="n">
         <v>50</v>
@@ -3389,7 +3389,7 @@
         </is>
       </c>
       <c r="D5" s="2" t="n">
-        <v>45937.21820112691</v>
+        <v>45937.22126852441</v>
       </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="n">
@@ -3424,10 +3424,10 @@
         </is>
       </c>
       <c r="D6" s="2" t="n">
-        <v>45937.2070900158</v>
+        <v>45937.2101574133</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>45937.2320900158</v>
+        <v>45937.2351574133</v>
       </c>
       <c r="F6" t="n">
         <v>55</v>
@@ -3856,7 +3856,7 @@
         </is>
       </c>
       <c r="D3" s="2" t="n">
-        <v>45937.23209003957</v>
+        <v>45937.23515743858</v>
       </c>
       <c r="E3" t="n">
         <v>45</v>
@@ -3907,7 +3907,7 @@
         </is>
       </c>
       <c r="D4" s="2" t="n">
-        <v>45937.23209003957</v>
+        <v>45937.23515743858</v>
       </c>
       <c r="E4" t="n">
         <v>42</v>
@@ -3958,7 +3958,7 @@
         </is>
       </c>
       <c r="D5" s="2" t="n">
-        <v>45937.23209003957</v>
+        <v>45937.23515743858</v>
       </c>
       <c r="E5" t="n">
         <v>38</v>
@@ -4009,7 +4009,7 @@
         </is>
       </c>
       <c r="D6" s="2" t="n">
-        <v>45937.23209003957</v>
+        <v>45937.23515743858</v>
       </c>
       <c r="E6" t="n">
         <v>48</v>
@@ -4060,7 +4060,7 @@
         </is>
       </c>
       <c r="D7" s="2" t="n">
-        <v>45937.23209003957</v>
+        <v>45937.23515743858</v>
       </c>
       <c r="E7" t="n">
         <v>35</v>

</xml_diff>

<commit_message>
Add comprehensive summary documentation for formula-based version
Co-authored-by: peetee09 <93839860+peetee09@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Ecom_Operations_Tracking_System_Formula_Based.xlsx
+++ b/Ecom_Operations_Tracking_System_Formula_Based.xlsx
@@ -928,7 +928,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>45937.23515745207</v>
+        <v>45937.23671582768</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -982,7 +982,7 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>45937.23515745207</v>
+        <v>45937.23671582768</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -1036,7 +1036,7 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>45937.23515745207</v>
+        <v>45937.23671582768</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -1090,7 +1090,7 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>45937.23515745207</v>
+        <v>45937.23671582768</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -1237,7 +1237,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>45937.23515746477</v>
+        <v>45937.23671583962</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -1287,7 +1287,7 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>45937.23515746477</v>
+        <v>45937.23671583962</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -1337,7 +1337,7 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>45937.23515746477</v>
+        <v>45937.23671583962</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -1387,7 +1387,7 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>45937.23515746477</v>
+        <v>45937.23671583962</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -1842,7 +1842,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>45937.23515733849</v>
+        <v>45937.23671571868</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -1870,7 +1870,7 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>45937.23515733849</v>
+        <v>45937.23671571868</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -1898,7 +1898,7 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>45937.23515733849</v>
+        <v>45937.23671571868</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -1926,7 +1926,7 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>45937.23515733849</v>
+        <v>45937.23671571868</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -1954,7 +1954,7 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>45937.23515733849</v>
+        <v>45937.23671571868</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -1982,7 +1982,7 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>45937.23515733849</v>
+        <v>45937.23671571868</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -2010,7 +2010,7 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>45937.23515733849</v>
+        <v>45937.23671571868</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -2125,13 +2125,13 @@
         </is>
       </c>
       <c r="B3" s="9" t="n">
-        <v>45937.193490685</v>
+        <v>45937.19504906513</v>
       </c>
       <c r="C3" s="9" t="n">
-        <v>45937.23515735166</v>
+        <v>45937.23671573179</v>
       </c>
       <c r="D3" s="9" t="n">
-        <v>45937.23168512945</v>
+        <v>45937.23324350957</v>
       </c>
       <c r="E3" s="10">
         <f>(D3-B3)*24*60</f>
@@ -2161,13 +2161,13 @@
         </is>
       </c>
       <c r="B4" s="9" t="n">
-        <v>45937.15182401834</v>
+        <v>45937.15338239846</v>
       </c>
       <c r="C4" s="9" t="n">
-        <v>45937.193490685</v>
+        <v>45937.19504906513</v>
       </c>
       <c r="D4" s="9" t="n">
-        <v>45937.19001846278</v>
+        <v>45937.1915768429</v>
       </c>
       <c r="E4" s="10">
         <f>(D4-B4)*24*60</f>
@@ -2197,10 +2197,10 @@
         </is>
       </c>
       <c r="B5" s="9" t="n">
-        <v>45937.21432401834</v>
+        <v>45937.21588239846</v>
       </c>
       <c r="C5" s="9" t="n">
-        <v>45937.255990685</v>
+        <v>45937.25754906513</v>
       </c>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
@@ -2228,10 +2228,10 @@
         </is>
       </c>
       <c r="B6" s="9" t="n">
-        <v>45937.224740685</v>
+        <v>45937.22629906513</v>
       </c>
       <c r="C6" s="9" t="n">
-        <v>45937.26640735166</v>
+        <v>45937.26796573179</v>
       </c>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
@@ -2752,7 +2752,7 @@
         <v>500</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>45937.13099071968</v>
+        <v>45937.13254909907</v>
       </c>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="n">
@@ -2795,10 +2795,10 @@
         <v>750</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>45937.16015738634</v>
+        <v>45937.16171576574</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>45937.23515738634</v>
+        <v>45937.23671576574</v>
       </c>
       <c r="I4" s="7">
         <f>(H4-G4)*24</f>
@@ -2841,7 +2841,7 @@
         <v>1000</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>45937.10182405301</v>
+        <v>45937.1033824324</v>
       </c>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="n">
@@ -2884,10 +2884,10 @@
         <v>600</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>45937.14765738634</v>
+        <v>45937.14921576574</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>45937.23515738634</v>
+        <v>45937.23671576574</v>
       </c>
       <c r="I6" s="7">
         <f>(H6-G6)*24</f>
@@ -3010,7 +3010,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>45937.23515740021</v>
+        <v>45937.23671577936</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -3055,7 +3055,7 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>45937.23515740021</v>
+        <v>45937.23671577936</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -3100,7 +3100,7 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>45937.23515740021</v>
+        <v>45937.23671577936</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -3145,7 +3145,7 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>45937.23515740021</v>
+        <v>45937.23671577936</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -3299,10 +3299,10 @@
         </is>
       </c>
       <c r="D3" s="2" t="n">
-        <v>45937.21571296886</v>
+        <v>45937.21727134697</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>45937.2351574133</v>
+        <v>45937.23671579141</v>
       </c>
       <c r="F3" t="n">
         <v>45</v>
@@ -3344,10 +3344,10 @@
         </is>
       </c>
       <c r="D4" s="2" t="n">
-        <v>45937.20876852441</v>
+        <v>45937.21032690252</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>45937.2351574133</v>
+        <v>45937.23671579141</v>
       </c>
       <c r="F4" t="n">
         <v>50</v>
@@ -3389,7 +3389,7 @@
         </is>
       </c>
       <c r="D5" s="2" t="n">
-        <v>45937.22126852441</v>
+        <v>45937.22282690252</v>
       </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="n">
@@ -3424,10 +3424,10 @@
         </is>
       </c>
       <c r="D6" s="2" t="n">
-        <v>45937.2101574133</v>
+        <v>45937.21171579141</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>45937.2351574133</v>
+        <v>45937.23671579141</v>
       </c>
       <c r="F6" t="n">
         <v>55</v>
@@ -3856,7 +3856,7 @@
         </is>
       </c>
       <c r="D3" s="2" t="n">
-        <v>45937.23515743858</v>
+        <v>45937.23671581491</v>
       </c>
       <c r="E3" t="n">
         <v>45</v>
@@ -3907,7 +3907,7 @@
         </is>
       </c>
       <c r="D4" s="2" t="n">
-        <v>45937.23515743858</v>
+        <v>45937.23671581491</v>
       </c>
       <c r="E4" t="n">
         <v>42</v>
@@ -3958,7 +3958,7 @@
         </is>
       </c>
       <c r="D5" s="2" t="n">
-        <v>45937.23515743858</v>
+        <v>45937.23671581491</v>
       </c>
       <c r="E5" t="n">
         <v>38</v>
@@ -4009,7 +4009,7 @@
         </is>
       </c>
       <c r="D6" s="2" t="n">
-        <v>45937.23515743858</v>
+        <v>45937.23671581491</v>
       </c>
       <c r="E6" t="n">
         <v>48</v>
@@ -4060,7 +4060,7 @@
         </is>
       </c>
       <c r="D7" s="2" t="n">
-        <v>45937.23515743858</v>
+        <v>45937.23671581491</v>
       </c>
       <c r="E7" t="n">
         <v>35</v>

</xml_diff>